<commit_message>
Fine tuned DBC merge and added value_tables
</commit_message>
<xml_diff>
--- a/scripts/Build Bus DBCs/CAN/Gauge Bus/Gauges.xlsx
+++ b/scripts/Build Bus DBCs/CAN/Gauge Bus/Gauges.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bollingermotors-my.sharepoint.com/personal/robert_bollingermotors_com/Documents/Bollinger/Engineering 3/80-Interior/Subsystems-Components/Gauges &amp; Msg Center Display/Riverside/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\core-controls\CAN\Gauge Bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{CA3EB42F-683E-4D36-964B-6B6CAE3B8ADB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{84B2DFE6-DF64-4BB3-9112-BBBCFBFF74F6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87A6D94-1D67-4D61-BDE0-3347D66B5A1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{CDFF86E9-28DD-4546-BF09-74B79B111AE9}"/>
   </bookViews>
@@ -398,9 +398,6 @@
     <t>Illuminate Charge Soon</t>
   </si>
   <si>
-    <t>Illuminate minate Battery Temp</t>
-  </si>
-  <si>
     <t>Illuminate Flat Tow</t>
   </si>
   <si>
@@ -447,6 +444,9 @@
   </si>
   <si>
     <t>0 - Off, 1 - Chime On, 2 - Reserved, 3 - Reserved</t>
+  </si>
+  <si>
+    <t>Illuminate Battery Temp</t>
   </si>
 </sst>
 </file>
@@ -829,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C07E074-2080-4950-8D9D-8A83A8E569B2}">
   <dimension ref="B2:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -941,7 +941,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="29" x14ac:dyDescent="0.35">
@@ -958,7 +958,7 @@
         <v>2</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="29" x14ac:dyDescent="0.35">
@@ -975,7 +975,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="29" x14ac:dyDescent="0.35">
@@ -992,7 +992,7 @@
         <v>2</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="29" x14ac:dyDescent="0.35">
@@ -1073,7 +1073,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="29" x14ac:dyDescent="0.35">
@@ -1090,7 +1090,7 @@
         <v>2</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="29" x14ac:dyDescent="0.35">
@@ -1107,7 +1107,7 @@
         <v>2</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="29" x14ac:dyDescent="0.35">
@@ -1124,7 +1124,7 @@
         <v>2</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="29" x14ac:dyDescent="0.35">
@@ -1141,7 +1141,7 @@
         <v>2</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="2:15" ht="29" x14ac:dyDescent="0.35">
@@ -1158,15 +1158,15 @@
         <v>2</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="29" x14ac:dyDescent="0.35">
       <c r="G16" t="s">
+        <v>134</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="I16">
         <v>28</v>
@@ -1175,7 +1175,7 @@
         <v>2</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1230,7 +1230,7 @@
         <v>2</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1247,15 +1247,15 @@
         <v>2</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="3:15" ht="58" x14ac:dyDescent="0.35">
       <c r="G20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I20">
         <v>32</v>
@@ -1264,7 +1264,7 @@
         <v>8</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1351,7 +1351,7 @@
         <v>2</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="3:15" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -1368,7 +1368,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="3:15" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -1385,7 +1385,7 @@
         <v>2</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1393,7 +1393,7 @@
         <v>20</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I26">
         <v>6</v>
@@ -1402,7 +1402,7 @@
         <v>2</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="3:15" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -1419,7 +1419,7 @@
         <v>2</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1427,7 +1427,7 @@
         <v>21</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I28">
         <v>10</v>
@@ -1436,7 +1436,7 @@
         <v>2</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1444,7 +1444,7 @@
         <v>26</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I29">
         <v>12</v>
@@ -1453,7 +1453,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1470,7 +1470,7 @@
         <v>2</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1478,7 +1478,7 @@
         <v>53</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I31">
         <v>16</v>
@@ -1487,7 +1487,7 @@
         <v>2</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1495,7 +1495,7 @@
         <v>52</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="I32">
         <v>18</v>
@@ -1504,7 +1504,7 @@
         <v>2</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1521,7 +1521,7 @@
         <v>2</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1538,7 +1538,7 @@
         <v>2</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1555,7 +1555,7 @@
         <v>2</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1572,7 +1572,7 @@
         <v>2</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1589,7 +1589,7 @@
         <v>2</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1606,15 +1606,15 @@
         <v>2</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="3:15" ht="58" x14ac:dyDescent="0.35">
       <c r="G39" t="s">
+        <v>130</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="I39">
         <v>32</v>
@@ -1623,7 +1623,7 @@
         <v>8</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="3:15" ht="29" x14ac:dyDescent="0.35">
@@ -1710,7 +1710,7 @@
         <v>0</v>
       </c>
       <c r="N42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O42" t="s">
         <v>93</v>
@@ -1736,7 +1736,7 @@
         <v>0</v>
       </c>
       <c r="N43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O43" t="s">
         <v>94</v>
@@ -1762,7 +1762,7 @@
         <v>-100</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O44" t="s">
         <v>92</v>
@@ -1788,7 +1788,7 @@
         <v>0</v>
       </c>
       <c r="N45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O45" t="s">
         <v>95</v>

</xml_diff>